<commit_message>
v0.39 Fixed IIC R/W bug and made Main GUI write to HW directly after any changes
</commit_message>
<xml_diff>
--- a/Documentation/Feedback & ToDoList/4711_GUI_FB_0.2.xlsx
+++ b/Documentation/Feedback & ToDoList/4711_GUI_FB_0.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>I2C Device Address加上</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,24 +117,6 @@
   </si>
   <si>
     <t>并修复刚打开时值没更新过了的bug</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sync 整个寄存器表还是只 Sync 主界面的寄存器值兵显示在界面上？
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A:sync是要把所有寄存器回读，然后更新到相应界面</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -295,6 +277,22 @@
   <si>
     <t>Noise-gate需要添加界面；
 增加类似DRC的图形界面(Threshold, attack/decay/hold time)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何Sync Mode Config？ 由很多寄存器组成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOne</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,7 +682,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -750,9 +748,11 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27">
@@ -764,7 +764,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="40.5">
@@ -778,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -801,16 +801,18 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="27">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -862,7 +864,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -888,7 +890,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27">
@@ -896,7 +898,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -912,7 +914,7 @@
         <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="27">
@@ -926,7 +928,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -948,9 +950,11 @@
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -968,9 +972,11 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
@@ -978,7 +984,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -988,7 +994,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -1000,9 +1006,11 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
@@ -1010,9 +1018,11 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
@@ -1020,9 +1030,11 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D28" s="2"/>
     </row>
   </sheetData>

</xml_diff>